<commit_message>
Se actualiza json de wordActivity
</commit_message>
<xml_diff>
--- a/WordActivity/Resources/Actividad-palabras.xlsx
+++ b/WordActivity/Resources/Actividad-palabras.xlsx
@@ -98,61 +98,145 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
-  <si>
-    <t>Palabras validas</t>
-  </si>
-  <si>
-    <t>Eres,tanta,gente,quién,ahora</t>
-  </si>
-  <si>
-    <t>Eres,ahora</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Nivel</t>
   </si>
   <si>
-    <t>Palabras a mostrar</t>
-  </si>
-  <si>
     <t>Canciones</t>
   </si>
   <si>
-    <t>alejandro sanz no es lo mismo</t>
-  </si>
-  <si>
-    <t>Eres-heres,tanta,gente,quién,ahora-hahora</t>
-  </si>
-  <si>
-    <t>Eres-heres,ahora-hahora</t>
-  </si>
-  <si>
-    <t>achi mamita kumari</t>
-  </si>
-  <si>
-    <t>aeroplano</t>
-  </si>
-  <si>
-    <t>charipany</t>
-  </si>
-  <si>
-    <t>kusa warmi</t>
-  </si>
-  <si>
-    <t>sumak warmi</t>
-  </si>
-  <si>
-    <t>telefono nucanchi nan</t>
-  </si>
-  <si>
-    <t>urpiku</t>
+    <t>HIWA</t>
+  </si>
+  <si>
+    <t>URPIKU</t>
+  </si>
+  <si>
+    <t>CHARIPANI</t>
+  </si>
+  <si>
+    <t>TELEFONO</t>
+  </si>
+  <si>
+    <t>Palabrasamostrar</t>
+  </si>
+  <si>
+    <t>Palabrasvalidas</t>
+  </si>
+  <si>
+    <t>traduccióndepalabras</t>
+  </si>
+  <si>
+    <t>Urpigu/Urpiku,ñabi/Ñawi,Jatun/Hatun,Wasi,Pay</t>
+  </si>
+  <si>
+    <t>Urpigu/Urpiku,ñabi/Ñawi</t>
+  </si>
+  <si>
+    <t>urpigo,(paloma),Ñabi,Rostro</t>
+  </si>
+  <si>
+    <t>Jiwa/Hiwa,Churo/Churu,Wagra,Puca/Puka,Ali/Alli</t>
+  </si>
+  <si>
+    <t>Jiwa/Hiwa,Churo/Churu</t>
+  </si>
+  <si>
+    <t>Jiwa(yerba,prado),Churu(Caracol)</t>
+  </si>
+  <si>
+    <t>Sumak,shungu/Shunku,Maki,Chaki,Shimi</t>
+  </si>
+  <si>
+    <t>Sumak,shungu/Shunku</t>
+  </si>
+  <si>
+    <t>SUMAKWARMI</t>
+  </si>
+  <si>
+    <t>Sumak,(bonita),Shunku(corazón)</t>
+  </si>
+  <si>
+    <t>Aeroplanuta,Puyu,Umasapa,Rin,Urco/Urku</t>
+  </si>
+  <si>
+    <t>Aeroplanuta,Puyu</t>
+  </si>
+  <si>
+    <t>AEROPLANO</t>
+  </si>
+  <si>
+    <t>Puyu(nube),aeroplanuta(elavión)</t>
+  </si>
+  <si>
+    <t>yanawagra/yanawakra,Kulki/Kullki,Pacari/Pakary,Kusa,Wañusca/Wañuska</t>
+  </si>
+  <si>
+    <t>yanawagra/yanawakra,Kulki/Kullki</t>
+  </si>
+  <si>
+    <t>yanawagra(vacanegra),kilku(dinero)</t>
+  </si>
+  <si>
+    <t>Tia,Ushi,Mama,Taita,Wambra</t>
+  </si>
+  <si>
+    <t>Tia,Ushi</t>
+  </si>
+  <si>
+    <t>TiaMamalla</t>
+  </si>
+  <si>
+    <t>Tia(Señora)Ushi(hija,niña)</t>
+  </si>
+  <si>
+    <t>Tushuy,Pacari/Pakari,Micuy,Ricuy/Rikuy,Munay</t>
+  </si>
+  <si>
+    <t>Tushuy,Pacari/Pakari</t>
+  </si>
+  <si>
+    <t>ACHIMAMITAKUMARI</t>
+  </si>
+  <si>
+    <t>Tushuy(Bailar),Pacari(Amanecer)</t>
+  </si>
+  <si>
+    <t>Warmi,Wacai/Wakay,Alcu/Alku,Ñucanchi,Sumak</t>
+  </si>
+  <si>
+    <t>Warmi,Wacai/Wakay</t>
+  </si>
+  <si>
+    <t>Wakay(triste),Warmi,Mujer</t>
+  </si>
+  <si>
+    <t>Sisakukuna/Sisagokuna,Sarakuta/Saragota,Kuchi,Wagra,Jiwa/Hiwa</t>
+  </si>
+  <si>
+    <t>Sisakukuna/Sisagokuna,Sarakuta/Saragota</t>
+  </si>
+  <si>
+    <t>KUSAWARMI</t>
+  </si>
+  <si>
+    <t>Sisakukuna(Florecitas),Sarakuta(Maicito)</t>
+  </si>
+  <si>
+    <t>Shimita,Ñan,Uma,Inti,Tuta</t>
+  </si>
+  <si>
+    <t>Shimita,Ñan</t>
+  </si>
+  <si>
+    <t>Shimi(laboca)Ñan(Camino</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,13 +259,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -215,11 +292,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -233,6 +308,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -525,172 +603,206 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>7</v>
+      <c r="B11" t="s">
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>